<commit_message>
multiple commands implementation and test cases
</commit_message>
<xml_diff>
--- a/Test data.xlsx
+++ b/Test data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="93">
   <si>
     <t>PLACE (2, 2, N)   </t>
   </si>
@@ -203,6 +203,96 @@
   </si>
   <si>
     <t>1,1,WEST</t>
+  </si>
+  <si>
+    <t>Place(2,3,S)</t>
+  </si>
+  <si>
+    <t>Move</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Move </t>
+  </si>
+  <si>
+    <t>Report</t>
+  </si>
+  <si>
+    <t>2,1 South</t>
+  </si>
+  <si>
+    <t>Place(1,1,E)</t>
+  </si>
+  <si>
+    <t>Left</t>
+  </si>
+  <si>
+    <t>LEFT</t>
+  </si>
+  <si>
+    <t>1,1,West</t>
+  </si>
+  <si>
+    <t>Place(1,2,N)</t>
+  </si>
+  <si>
+    <t>Right</t>
+  </si>
+  <si>
+    <t>1,2, SOUTH</t>
+  </si>
+  <si>
+    <t>Place(3,3,W)</t>
+  </si>
+  <si>
+    <t>Place(2,1,E)</t>
+  </si>
+  <si>
+    <t>2,1 EAST</t>
+  </si>
+  <si>
+    <t>Place(1,2,S)</t>
+  </si>
+  <si>
+    <t>2,2, EAST</t>
+  </si>
+  <si>
+    <t>PLACE(2,3,N)</t>
+  </si>
+  <si>
+    <t>3,3,EAST</t>
+  </si>
+  <si>
+    <t>PLACE(4,4,w)</t>
+  </si>
+  <si>
+    <t>3,4,SOUTH</t>
+  </si>
+  <si>
+    <t>PLACE(2,3,E)</t>
+  </si>
+  <si>
+    <t>3,3,SOUTH</t>
+  </si>
+  <si>
+    <t>1,2 NORTH</t>
+  </si>
+  <si>
+    <t>PLACE(3,2,s)</t>
+  </si>
+  <si>
+    <t>3,2,SOUTH</t>
+  </si>
+  <si>
+    <t>PLACE(3,4,N)</t>
+  </si>
+  <si>
+    <t>PLACE(2,1,S)</t>
+  </si>
+  <si>
+    <t>Place(1,2,E)</t>
+  </si>
+  <si>
+    <t>3,5,EAST</t>
   </si>
 </sst>
 </file>
@@ -644,10 +734,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G112"/>
+  <dimension ref="A1:G175"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A101" workbookViewId="0">
-      <selection activeCell="E124" sqref="E124"/>
+    <sheetView tabSelected="1" topLeftCell="A152" workbookViewId="0">
+      <selection activeCell="E162" sqref="E162"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1344,6 +1434,384 @@
       </c>
       <c r="C112" s="7"/>
     </row>
+    <row r="113" spans="1:3" ht="15.75" thickBot="1"/>
+    <row r="114" spans="1:3">
+      <c r="A114">
+        <v>19</v>
+      </c>
+      <c r="B114" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C114" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3">
+      <c r="B115" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C115" s="5"/>
+    </row>
+    <row r="116" spans="1:3">
+      <c r="B116" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C116" s="5"/>
+    </row>
+    <row r="117" spans="1:3" ht="15.75" thickBot="1">
+      <c r="B117" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="C117" s="7"/>
+    </row>
+    <row r="118" spans="1:3" ht="15.75" thickBot="1"/>
+    <row r="119" spans="1:3">
+      <c r="A119">
+        <v>20</v>
+      </c>
+      <c r="B119" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C119" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3">
+      <c r="B120" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C120" s="5"/>
+    </row>
+    <row r="121" spans="1:3">
+      <c r="B121" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C121" s="5"/>
+    </row>
+    <row r="122" spans="1:3" ht="15.75" thickBot="1">
+      <c r="B122" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="C122" s="7"/>
+    </row>
+    <row r="123" spans="1:3" ht="15.75" thickBot="1"/>
+    <row r="124" spans="1:3">
+      <c r="A124">
+        <v>21</v>
+      </c>
+      <c r="B124" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C124" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3">
+      <c r="B125" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C125" s="5"/>
+    </row>
+    <row r="126" spans="1:3">
+      <c r="B126" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C126" s="5"/>
+    </row>
+    <row r="127" spans="1:3" ht="15.75" thickBot="1">
+      <c r="B127" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C127" s="7"/>
+    </row>
+    <row r="128" spans="1:3" ht="15.75" thickBot="1"/>
+    <row r="129" spans="1:3">
+      <c r="A129">
+        <v>22</v>
+      </c>
+      <c r="B129" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C129" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3">
+      <c r="B130" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C130" s="5"/>
+    </row>
+    <row r="131" spans="1:3" ht="15.75" thickBot="1">
+      <c r="B131" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="C131" s="7"/>
+    </row>
+    <row r="132" spans="1:3" ht="15.75" thickBot="1"/>
+    <row r="133" spans="1:3">
+      <c r="A133">
+        <v>23</v>
+      </c>
+      <c r="B133" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C133" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3">
+      <c r="B134" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C134" s="5"/>
+    </row>
+    <row r="135" spans="1:3">
+      <c r="B135" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C135" s="5"/>
+    </row>
+    <row r="136" spans="1:3" ht="15.75" thickBot="1">
+      <c r="B136" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C136" s="7"/>
+    </row>
+    <row r="137" spans="1:3" ht="15.75" thickBot="1"/>
+    <row r="138" spans="1:3">
+      <c r="A138">
+        <v>24</v>
+      </c>
+      <c r="B138" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C138" s="3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3">
+      <c r="B139" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C139" s="5"/>
+    </row>
+    <row r="140" spans="1:3">
+      <c r="B140" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C140" s="5"/>
+    </row>
+    <row r="141" spans="1:3" ht="15.75" thickBot="1">
+      <c r="B141" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C141" s="7"/>
+    </row>
+    <row r="142" spans="1:3" ht="15.75" thickBot="1"/>
+    <row r="143" spans="1:3">
+      <c r="A143">
+        <v>25</v>
+      </c>
+      <c r="B143" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C143" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3">
+      <c r="B144" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C144" s="5"/>
+    </row>
+    <row r="145" spans="1:3">
+      <c r="B145" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C145" s="5"/>
+    </row>
+    <row r="146" spans="1:3" ht="15.75" thickBot="1">
+      <c r="B146" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C146" s="7"/>
+    </row>
+    <row r="147" spans="1:3" ht="15.75" thickBot="1"/>
+    <row r="148" spans="1:3">
+      <c r="A148">
+        <v>26</v>
+      </c>
+      <c r="B148" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C148" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3">
+      <c r="B149" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C149" s="5"/>
+    </row>
+    <row r="150" spans="1:3">
+      <c r="B150" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C150" s="5"/>
+    </row>
+    <row r="151" spans="1:3" ht="15.75" thickBot="1">
+      <c r="B151" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C151" s="7"/>
+    </row>
+    <row r="152" spans="1:3" ht="15.75" thickBot="1"/>
+    <row r="153" spans="1:3">
+      <c r="A153">
+        <v>27</v>
+      </c>
+      <c r="B153" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C153" s="3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3">
+      <c r="B154" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C154" s="5"/>
+    </row>
+    <row r="155" spans="1:3">
+      <c r="B155" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C155" s="5"/>
+    </row>
+    <row r="156" spans="1:3" ht="15.75" thickBot="1">
+      <c r="B156" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C156" s="7"/>
+    </row>
+    <row r="157" spans="1:3" ht="15.75" thickBot="1"/>
+    <row r="158" spans="1:3">
+      <c r="A158">
+        <v>28</v>
+      </c>
+      <c r="B158" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C158" s="3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="159" spans="1:3">
+      <c r="B159" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C159" s="5"/>
+    </row>
+    <row r="160" spans="1:3">
+      <c r="B160" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C160" s="5"/>
+    </row>
+    <row r="161" spans="1:3" ht="15.75" thickBot="1">
+      <c r="B161" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C161" s="7"/>
+    </row>
+    <row r="162" spans="1:3" ht="15.75" thickBot="1"/>
+    <row r="163" spans="1:3">
+      <c r="A163">
+        <v>29</v>
+      </c>
+      <c r="B163" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C163" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3">
+      <c r="B164" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C164" s="5"/>
+    </row>
+    <row r="165" spans="1:3">
+      <c r="B165" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="C165" s="5"/>
+    </row>
+    <row r="166" spans="1:3">
+      <c r="B166" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C166" s="5"/>
+    </row>
+    <row r="167" spans="1:3">
+      <c r="B167" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C167" s="5"/>
+    </row>
+    <row r="168" spans="1:3" ht="15.75" thickBot="1">
+      <c r="B168" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C168" s="7"/>
+    </row>
+    <row r="169" spans="1:3" ht="15.75" thickBot="1"/>
+    <row r="170" spans="1:3">
+      <c r="A170">
+        <v>30</v>
+      </c>
+      <c r="B170" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C170" s="3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="171" spans="1:3">
+      <c r="B171" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C171" s="5"/>
+    </row>
+    <row r="172" spans="1:3">
+      <c r="B172" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="C172" s="5"/>
+    </row>
+    <row r="173" spans="1:3">
+      <c r="B173" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C173" s="5"/>
+    </row>
+    <row r="174" spans="1:3">
+      <c r="B174" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C174" s="5"/>
+    </row>
+    <row r="175" spans="1:3" ht="15.75" thickBot="1">
+      <c r="B175" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C175" s="7"/>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="F2:G3"/>

</xml_diff>